<commit_message>
corrected 31 ppm pH
</commit_message>
<xml_diff>
--- a/logs/hoagland_ph_weekly.xlsx
+++ b/logs/hoagland_ph_weekly.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaara\Documents\github\2025_g34p\logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monik\Documents\git\2025_g34p\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D0D3E9-588F-4C43-A5E1-3303D5C3E83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09B6276-3424-4F82-860B-C3756EB62357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{8D8DBED7-4830-46A9-B76D-E0096B6445E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D8DBED7-4830-46A9-B76D-E0096B6445E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>hoagland solution fertilizer weekly pH</t>
   </si>
@@ -74,13 +74,10 @@
     <t>week 05</t>
   </si>
   <si>
-    <t>6.87*</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>*Overfilled by 675 mL</t>
+    <t xml:space="preserve">*Overfilled by 675 mL on 08/15/2025. pH was 6.87, corrected by adding extra nut. On 08/18/2025, new pH. </t>
   </si>
 </sst>
 </file>
@@ -122,10 +119,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,24 +456,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E599DF-0674-4691-8FF2-730716D2E8B0}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.86328125" customWidth="1"/>
-    <col min="2" max="2" width="13.1328125" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -488,7 +484,7 @@
         <v>45884</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -508,7 +504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -519,7 +515,7 @@
         <v>6.37</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -530,18 +526,18 @@
         <v>7.01</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8">
         <v>6.7</v>
       </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="C8">
+        <v>6.96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -552,16 +548,13 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>